<commit_message>
Updated ITA_grids model - 2025-08-19 22:52
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA_grids/SuppXLS/scen_tsparameters_triple_1.xlsx
+++ b/VerveStacks_ITA_grids/SuppXLS/scen_tsparameters_triple_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA_grids\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D924E195-F642-4510-B598-BEEA4EC5FE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4CF2E53-C3E4-402F-8809-A3F4BE665FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -900,10 +900,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>S1aH5,S1b0202h07,S2aH4,S2aH5,S2c0304h17,S4d1024h16,S5aH2,S5aH5,S1aH4,S1b0202h12,S2aH2,S2c0304h11,S4d1024h17,S2c0304h16,S2c0304h12,S2c0304h13,S2c0304h14,S4aH5,S1b0202h09,S4d1024h15,S2c0304h08,S4aH2,S4d1024h07,S1b0202h08,S1b0202h11,S3aH2,S4d1024h09,S1b0202h15,S2c0304h18,S3aH3,S1b0202h10,S1b0202h18,S3aH4,S4aH3,S4aH4,S4d1024h11,S1b0202h14,S3aH5,S4d1024h13,S4d1024h18,S5aH3,S1aH3,S4d1024h12,S4d1024h14,S4d1024h08,S4d1024h10,S1b0202h13,S1b0202h16,S2c0304h09,S5aH4,S1aH2,S1b0202h17,S2aH3,S2c0304h10,S2c0304h15,S2c0304h07</t>
-  </si>
-  <si>
-    <t>S1aH6,S1b0202h05,S1b0202h06,S2c0304h24,S4d1024h01,S2c0304h04,S2c0304h22,S4aH1,S4d1024h24,S1aH1,S1b0202h20,S1b0202h23,S2aH7,S4d1024h20,S4d1024h22,S2c0304h05,S4d1024h23,S1b0202h04,S2c0304h01,S4aH8,S1b0202h03,S1b0202h22,S2aH1,S2c0304h02,S3aH7,S4d1024h02,S4d1024h06,S5aH8,S1b0202h02,S1b0202h21,S2aH8,S4d1024h04,S1b0202h24,S2c0304h20,S3aH8,S1b0202h01,S2c0304h19,S4aH6,S4d1024h21,S2c0304h06,S4d1024h19,S1aH8,S5aH1,S1aH7,S2c0304h21,S3aH6,S4aH7,S5aH6,S5aH7,S2c0304h03,S2c0304h23,S4d1024h03,S4d1024h05,S1b0202h19,S2aH6,S3aH1</t>
+    <t>S4d1024h07,S1b0202h13,S1b0202h16,S2c0304h09,S5aH4,S1aH4,S1b0202h12,S2aH2,S2c0304h11,S4d1024h17,S1aH5,S1b0202h07,S2aH4,S2aH5,S2c0304h17,S4d1024h16,S5aH2,S5aH5,S1b0202h14,S3aH5,S4d1024h13,S4d1024h18,S5aH3,S1aH2,S1b0202h17,S2aH3,S2c0304h10,S2c0304h15,S2c0304h07,S1b0202h15,S2c0304h18,S3aH3,S2c0304h12,S2c0304h13,S2c0304h14,S4aH5,S4d1024h08,S4d1024h10,S1b0202h08,S1b0202h11,S3aH2,S4d1024h09,S2c0304h16,S1b0202h10,S1b0202h18,S3aH4,S4aH3,S4aH4,S4d1024h11,S1b0202h09,S4d1024h15,S2c0304h08,S4aH2,S1aH3,S4d1024h12,S4d1024h14</t>
+  </si>
+  <si>
+    <t>S1b0202h02,S1b0202h21,S2aH8,S4d1024h04,S4d1024h03,S2c0304h04,S2c0304h22,S4aH1,S4d1024h24,S1aH6,S1b0202h05,S1b0202h06,S2c0304h24,S4d1024h01,S1aH8,S5aH1,S4d1024h05,S1b0202h19,S2aH6,S3aH1,S1b0202h01,S2c0304h19,S4aH6,S4d1024h21,S2c0304h05,S4d1024h23,S2c0304h03,S2c0304h23,S1b0202h24,S2c0304h20,S3aH8,S1aH1,S1b0202h20,S1b0202h23,S2aH7,S4d1024h20,S4d1024h22,S2c0304h06,S4d1024h19,S1b0202h04,S2c0304h01,S4aH8,S1b0202h03,S1b0202h22,S2aH1,S2c0304h02,S3aH7,S4d1024h02,S4d1024h06,S5aH8,S1aH7,S2c0304h21,S3aH6,S4aH7,S5aH6,S5aH7</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1475,7 +1475,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>S1aH6,S1b0202h05,S1b0202h06,S2c0304h24,S4d1024h01,S2c0304h04,S2c0304h22,S4aH1,S4d1024h24,S1aH1,S1b0202h20,S1b0202h23,S2aH7,S4d1024h20,S4d1024h22,S2c0304h05,S4d1024h23,S1b0202h04,S2c0304h01,S4aH8,S1b0202h03,S1b0202h22,S2aH1,S2c0304h02,S3aH7,S4d1024h02,S4d1024h06,S5aH8,S1b0202h02,S1b0202h21,S2aH8,S4d1024h04,S1b0202h24,S2c0304h20,S3aH8,S1b0202h01,S2c0304h19,S4aH6,S4d1024h21,S2c0304h06,S4d1024h19,S1aH8,S5aH1,S1aH7,S2c0304h21,S3aH6,S4aH7,S5aH6,S5aH7,S2c0304h03,S2c0304h23,S4d1024h03,S4d1024h05,S1b0202h19,S2aH6,S3aH1</v>
+        <v>S1b0202h02,S1b0202h21,S2aH8,S4d1024h04,S4d1024h03,S2c0304h04,S2c0304h22,S4aH1,S4d1024h24,S1aH6,S1b0202h05,S1b0202h06,S2c0304h24,S4d1024h01,S1aH8,S5aH1,S4d1024h05,S1b0202h19,S2aH6,S3aH1,S1b0202h01,S2c0304h19,S4aH6,S4d1024h21,S2c0304h05,S4d1024h23,S2c0304h03,S2c0304h23,S1b0202h24,S2c0304h20,S3aH8,S1aH1,S1b0202h20,S1b0202h23,S2aH7,S4d1024h20,S4d1024h22,S2c0304h06,S4d1024h19,S1b0202h04,S2c0304h01,S4aH8,S1b0202h03,S1b0202h22,S2aH1,S2c0304h02,S3aH7,S4d1024h02,S4d1024h06,S5aH8,S1aH7,S2c0304h21,S3aH6,S4aH7,S5aH6,S5aH7</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1507,7 +1507,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>S1aH5,S1b0202h07,S2aH4,S2aH5,S2c0304h17,S4d1024h16,S5aH2,S5aH5,S1aH4,S1b0202h12,S2aH2,S2c0304h11,S4d1024h17,S2c0304h16,S2c0304h12,S2c0304h13,S2c0304h14,S4aH5,S1b0202h09,S4d1024h15,S2c0304h08,S4aH2,S4d1024h07,S1b0202h08,S1b0202h11,S3aH2,S4d1024h09,S1b0202h15,S2c0304h18,S3aH3,S1b0202h10,S1b0202h18,S3aH4,S4aH3,S4aH4,S4d1024h11,S1b0202h14,S3aH5,S4d1024h13,S4d1024h18,S5aH3,S1aH3,S4d1024h12,S4d1024h14,S4d1024h08,S4d1024h10,S1b0202h13,S1b0202h16,S2c0304h09,S5aH4,S1aH2,S1b0202h17,S2aH3,S2c0304h10,S2c0304h15,S2c0304h07</v>
+        <v>S4d1024h07,S1b0202h13,S1b0202h16,S2c0304h09,S5aH4,S1aH4,S1b0202h12,S2aH2,S2c0304h11,S4d1024h17,S1aH5,S1b0202h07,S2aH4,S2aH5,S2c0304h17,S4d1024h16,S5aH2,S5aH5,S1b0202h14,S3aH5,S4d1024h13,S4d1024h18,S5aH3,S1aH2,S1b0202h17,S2aH3,S2c0304h10,S2c0304h15,S2c0304h07,S1b0202h15,S2c0304h18,S3aH3,S2c0304h12,S2c0304h13,S2c0304h14,S4aH5,S4d1024h08,S4d1024h10,S1b0202h08,S1b0202h11,S3aH2,S4d1024h09,S2c0304h16,S1b0202h10,S1b0202h18,S3aH4,S4aH3,S4aH4,S4d1024h11,S1b0202h09,S4d1024h15,S2c0304h08,S4aH2,S1aH3,S4d1024h12,S4d1024h14</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2120,7 +2120,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABCFEF82-01F3-46D8-A91D-B178385B7096}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD7714E-1531-4D98-9071-D2C57FA1371E}">
   <dimension ref="B2:F83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2834,7 +2834,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6D6C932-6070-4A44-AACF-284BB96998BD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37D52806-665D-48D1-9D00-D924A42373E6}">
   <dimension ref="B2:O115"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2913,10 +2913,10 @@
         <v>282</v>
       </c>
       <c r="M4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="N4">
-        <v>0.16266774641369736</v>
+        <v>0.63189495603887091</v>
       </c>
       <c r="O4" t="s">
         <v>293</v>
@@ -2948,10 +2948,10 @@
         <v>282</v>
       </c>
       <c r="M5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="N5">
-        <v>0.18220731142989358</v>
+        <v>7.5520592318371119E-2</v>
       </c>
       <c r="O5" t="s">
         <v>293</v>
@@ -2983,10 +2983,10 @@
         <v>282</v>
       </c>
       <c r="M6" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="N6">
-        <v>0.63189495603887091</v>
+        <v>0.16266774641369736</v>
       </c>
       <c r="O6" t="s">
         <v>293</v>
@@ -3018,10 +3018,10 @@
         <v>282</v>
       </c>
       <c r="M7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="N7">
-        <v>7.5520592318371119E-2</v>
+        <v>0.14770939379916706</v>
       </c>
       <c r="O7" t="s">
         <v>293</v>
@@ -3053,10 +3053,10 @@
         <v>282</v>
       </c>
       <c r="M8" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="N8">
-        <v>0.14770939379916706</v>
+        <v>0.18220731142989358</v>
       </c>
       <c r="O8" t="s">
         <v>293</v>
@@ -5850,7 +5850,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B1EBD0-9E13-441A-BA53-0885BC3D23B9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D00EEC36-1F49-4D42-8BEE-B34A07FC2E00}">
   <dimension ref="B2:O227"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>